<commit_message>
Update SBA Science Variable Dictionary.xlsx
</commit_message>
<xml_diff>
--- a/SBA Science Variable Dictionary.xlsx
+++ b/SBA Science Variable Dictionary.xlsx
@@ -391,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -516,21 +516,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -577,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -615,9 +600,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -921,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +921,7 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -958,14 +940,14 @@
       <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -984,15 +966,17 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1008,11 +992,11 @@
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
@@ -1027,11 +1011,11 @@
         <v>97</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -1046,11 +1030,11 @@
       <c r="F5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -1065,11 +1049,11 @@
         <v>99</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -1084,11 +1068,11 @@
       <c r="F7" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1103,11 +1087,11 @@
         <v>14</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -1120,11 +1104,11 @@
         <v>16</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>17</v>
@@ -1137,11 +1121,11 @@
         <v>18</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1156,11 +1140,11 @@
         <v>20</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -1175,11 +1159,11 @@
       <c r="F12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>100</v>
@@ -1196,13 +1180,13 @@
       <c r="F13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>101</v>
@@ -1219,11 +1203,11 @@
       <c r="F14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>25</v>
@@ -1238,13 +1222,13 @@
       <c r="F15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>26</v>
@@ -1259,11 +1243,11 @@
       <c r="F16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -1278,11 +1262,11 @@
       <c r="F17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>32</v>
@@ -1297,11 +1281,11 @@
       <c r="F18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>39</v>
@@ -1316,11 +1300,11 @@
       <c r="F19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>41</v>
@@ -1335,13 +1319,13 @@
       <c r="F20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>43</v>
@@ -1356,13 +1340,13 @@
       <c r="F21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
@@ -1377,11 +1361,11 @@
       <c r="F22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>47</v>
@@ -1396,11 +1380,11 @@
       <c r="F23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>49</v>
@@ -1415,11 +1399,11 @@
       <c r="F24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>51</v>
@@ -1434,11 +1418,11 @@
       <c r="F25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>53</v>
@@ -1453,11 +1437,11 @@
       <c r="F26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>89</v>
@@ -1472,11 +1456,11 @@
       <c r="F27" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>55</v>
@@ -1491,11 +1475,11 @@
       <c r="F28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>56</v>
@@ -1508,11 +1492,11 @@
         <v>59</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>57</v>
@@ -1527,11 +1511,11 @@
       <c r="F30" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>61</v>
@@ -1546,11 +1530,11 @@
       <c r="F31" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="15"/>
+    </row>
+    <row r="32" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>91</v>
@@ -1563,11 +1547,11 @@
       <c r="F32" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>63</v>
@@ -1582,26 +1566,26 @@
       <c r="F33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7" s="17" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
-        <v>32</v>
-      </c>
-      <c r="B34" s="12" t="s">
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="1:7" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="12" t="s">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="18"/>
+      <c r="G34" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>